<commit_message>
Added reference to original video
</commit_message>
<xml_diff>
--- a/GermanStoryNewWords.xlsx
+++ b/GermanStoryNewWords.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28407"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2CB219DC-7289-4F71-B82F-05D5CEDB8CC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82BAB59A-91DA-4959-A6BC-F60D61EE1EBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -30,6 +30,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -2478,7 +2480,7 @@
   </sheetPr>
   <dimension ref="A1:AF929"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="Z21" sqref="Z21"/>
     </sheetView>
   </sheetViews>
@@ -2517,7 +2519,7 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>01-Dec-2024</v>
+        <v>23-Dec-2024</v>
       </c>
       <c r="C3" s="2"/>
     </row>

</xml_diff>